<commit_message>
add some vocab unit 1 to english
</commit_message>
<xml_diff>
--- a/english/VOCAB_Unit1.xlsx
+++ b/english/VOCAB_Unit1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tutorials\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874716F6-0A31-4730-9225-C70DDC53B1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1182E680-1DF7-4471-80AC-BE7D4F3F803E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
   <si>
     <t>حماية البيئة/الصيانة/الحفاظ على</t>
   </si>
@@ -546,6 +546,171 @@
   </si>
   <si>
     <t>stuck(adj)</t>
+  </si>
+  <si>
+    <t>مفامرة</t>
+  </si>
+  <si>
+    <t>مريع/فظيع</t>
+  </si>
+  <si>
+    <t>متألق/ذكي</t>
+  </si>
+  <si>
+    <t>قلعة</t>
+  </si>
+  <si>
+    <t>castle(n)</t>
+  </si>
+  <si>
+    <t>brilliant(adj)</t>
+  </si>
+  <si>
+    <t>awful(adj)</t>
+  </si>
+  <si>
+    <t>adventure(n)</t>
+  </si>
+  <si>
+    <t>actually(adv)</t>
+  </si>
+  <si>
+    <t>cheap(adj)</t>
+  </si>
+  <si>
+    <t>cruise(n)</t>
+  </si>
+  <si>
+    <t>رخيص</t>
+  </si>
+  <si>
+    <t>رحلة بحرية</t>
+  </si>
+  <si>
+    <t>damage(d)(v - n)</t>
+  </si>
+  <si>
+    <t>distance(n)</t>
+  </si>
+  <si>
+    <t>مسافة</t>
+  </si>
+  <si>
+    <t>expect(ed)(v)</t>
+  </si>
+  <si>
+    <t>explore(d)(v)</t>
+  </si>
+  <si>
+    <t>يتوقع</t>
+  </si>
+  <si>
+    <t>يستكشف</t>
+  </si>
+  <si>
+    <t>fascinating(adj)</t>
+  </si>
+  <si>
+    <t>جذاب/فاتن</t>
+  </si>
+  <si>
+    <t>gardening(n)</t>
+  </si>
+  <si>
+    <t>بستنة</t>
+  </si>
+  <si>
+    <t>glad(adj)</t>
+  </si>
+  <si>
+    <t>مسرور</t>
+  </si>
+  <si>
+    <t>grow-grew-grown(v)</t>
+  </si>
+  <si>
+    <t>ينمو</t>
+  </si>
+  <si>
+    <t>guide(d)(n - v)</t>
+  </si>
+  <si>
+    <t>مرشد</t>
+  </si>
+  <si>
+    <t>on board</t>
+  </si>
+  <si>
+    <t>على متن السفينة</t>
+  </si>
+  <si>
+    <t>paradise(n)</t>
+  </si>
+  <si>
+    <t>جَنَّة</t>
+  </si>
+  <si>
+    <t>منتجع</t>
+  </si>
+  <si>
+    <t>resort(n)</t>
+  </si>
+  <si>
+    <t>sight</t>
+  </si>
+  <si>
+    <t>مشهد/احد المعالم</t>
+  </si>
+  <si>
+    <t>steal-stole-stolen(v)</t>
+  </si>
+  <si>
+    <t>يسرق</t>
+  </si>
+  <si>
+    <t>stressed(adj)</t>
+  </si>
+  <si>
+    <t>مضغوط</t>
+  </si>
+  <si>
+    <t>teenager(adj - n)</t>
+  </si>
+  <si>
+    <t>مراهق</t>
+  </si>
+  <si>
+    <t>tiny(adj)</t>
+  </si>
+  <si>
+    <t>صغير الحجم</t>
+  </si>
+  <si>
+    <t>underwater(adj-adv)</t>
+  </si>
+  <si>
+    <t>تحت الماء</t>
+  </si>
+  <si>
+    <t>unusual(adj)</t>
+  </si>
+  <si>
+    <t>غير عادي</t>
+  </si>
+  <si>
+    <t>يقلق</t>
+  </si>
+  <si>
+    <t>worry(ied)(n-v)</t>
+  </si>
+  <si>
+    <t>في الحقيقة/في الواقع</t>
+  </si>
+  <si>
+    <t>insulated(adj)</t>
+  </si>
+  <si>
+    <t>معزول</t>
   </si>
 </sst>
 </file>
@@ -863,16 +1028,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -905,6 +1070,30 @@
       </c>
       <c r="B4" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B7" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -918,7 +1107,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -930,7 +1119,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -944,7 +1133,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1003,7 +1192,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1037,7 +1226,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1054,15 +1243,15 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C0C726-EF5B-4FC9-82F4-48A94ABEDF76}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1098,6 +1287,14 @@
         <v>151</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B5" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1105,13 +1302,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A7C8CB-6C90-4DBF-A892-A597E3AA4FFB}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -1181,6 +1378,14 @@
         <v>155</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1194,7 +1399,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1214,13 +1419,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD8CC-E8BB-4467-BDFA-859B668822CD}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -1266,6 +1471,14 @@
         <v>163</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1273,13 +1486,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC3E5B7-A644-40B3-9FA0-0F3184C0C666}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -1349,6 +1562,30 @@
         <v>164</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1356,13 +1593,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853577DC-45D1-47FB-8CE1-2701635EB942}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1407,6 +1644,14 @@
         <v>130</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>171</v>
+      </c>
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1414,15 +1659,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB031BE2-8873-4BBE-A6E2-D6DA83495605}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1434,6 +1679,22 @@
         <v>29</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1441,13 +1702,16 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B0D9507-6158-4A9D-A406-C80DC24CA4EA}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1455,6 +1719,22 @@
       </c>
       <c r="B1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1470,7 +1750,7 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1506,13 +1786,16 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBD34EC-97FD-4DAA-AEDA-1EA3B169E39D}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1520,6 +1803,14 @@
       </c>
       <c r="B1" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1533,7 +1824,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1541,13 +1832,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22D18F6-24F4-4B6D-89D6-327046526B24}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
@@ -1617,6 +1908,30 @@
         <v>137</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>175</v>
+      </c>
+      <c r="B10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1624,13 +1939,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620BC664-2145-4DF7-8DD0-BC60C18F3A8C}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -1676,6 +1991,22 @@
         <v>57</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
+        <v>181</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1683,13 +2014,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED53159-19AE-4D6E-99FF-244D3305644D}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
@@ -1791,6 +2122,22 @@
         <v>139</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B14" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1798,15 +2145,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE4078B-C3FB-4387-BB88-A48544D11CEB}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1818,6 +2165,14 @@
         <v>101</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>187</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1825,15 +2180,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C90A18-1FDE-4DAE-9E49-D28AE616AC3A}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1842,6 +2197,38 @@
       </c>
       <c r="B1" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1857,7 +2244,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1885,13 +2272,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE4CAFB-C354-4385-8BA3-69100390E382}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1937,6 +2324,14 @@
         <v>109</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>219</v>
+      </c>
+      <c r="B6" t="s">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add unit 1 to english
</commit_message>
<xml_diff>
--- a/english/VOCAB_Unit1.xlsx
+++ b/english/VOCAB_Unit1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tutorials\english\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1182E680-1DF7-4471-80AC-BE7D4F3F803E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A4970D-AC4A-4A3E-9C56-97D5CA04B9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="381">
   <si>
     <t>حماية البيئة/الصيانة/الحفاظ على</t>
   </si>
@@ -665,9 +665,6 @@
     <t>steal-stole-stolen(v)</t>
   </si>
   <si>
-    <t>يسرق</t>
-  </si>
-  <si>
     <t>stressed(adj)</t>
   </si>
   <si>
@@ -711,6 +708,489 @@
   </si>
   <si>
     <t>معزول</t>
+  </si>
+  <si>
+    <t>admired(d)(v)</t>
+  </si>
+  <si>
+    <t>ability(n)</t>
+  </si>
+  <si>
+    <t>amongst(prep)</t>
+  </si>
+  <si>
+    <t>قدرة</t>
+  </si>
+  <si>
+    <t>يُعجَب ب</t>
+  </si>
+  <si>
+    <t>بين</t>
+  </si>
+  <si>
+    <t>agreement(n)</t>
+  </si>
+  <si>
+    <t>اتفاق</t>
+  </si>
+  <si>
+    <t>based in</t>
+  </si>
+  <si>
+    <t>benefit(ted)(n-v)</t>
+  </si>
+  <si>
+    <t>biography(n)</t>
+  </si>
+  <si>
+    <t>blood donation(n)</t>
+  </si>
+  <si>
+    <t>blood pressure(n)</t>
+  </si>
+  <si>
+    <t>تعتمد على/مقرها في</t>
+  </si>
+  <si>
+    <t>فائدة</t>
+  </si>
+  <si>
+    <t>سيرة شخصية</t>
+  </si>
+  <si>
+    <t>تبرع بالدم</t>
+  </si>
+  <si>
+    <t>ضغط الدم</t>
+  </si>
+  <si>
+    <t>chance(n)</t>
+  </si>
+  <si>
+    <t>charity(n)</t>
+  </si>
+  <si>
+    <t>check(ed)(v)</t>
+  </si>
+  <si>
+    <t>compassion(n)</t>
+  </si>
+  <si>
+    <t>cute(adj)</t>
+  </si>
+  <si>
+    <t>فرصة</t>
+  </si>
+  <si>
+    <t>صدقة/الاعمال الخيرية</t>
+  </si>
+  <si>
+    <t>يفحص/تحقق</t>
+  </si>
+  <si>
+    <t>عطف/شفقة</t>
+  </si>
+  <si>
+    <t>لطيف/جذاب</t>
+  </si>
+  <si>
+    <t>documentary(n-adj)</t>
+  </si>
+  <si>
+    <t>desire(d)(n-v)</t>
+  </si>
+  <si>
+    <t>donate(d)(v)</t>
+  </si>
+  <si>
+    <t>donation(n)</t>
+  </si>
+  <si>
+    <t>donor(n)</t>
+  </si>
+  <si>
+    <t>وثائقي</t>
+  </si>
+  <si>
+    <t>يرغب</t>
+  </si>
+  <si>
+    <t>يتبرع</t>
+  </si>
+  <si>
+    <t>تبرع</t>
+  </si>
+  <si>
+    <t>متبرع</t>
+  </si>
+  <si>
+    <t>finals(n)</t>
+  </si>
+  <si>
+    <t>fondness(n)</t>
+  </si>
+  <si>
+    <t>founder(n)</t>
+  </si>
+  <si>
+    <t>نهائيات</t>
+  </si>
+  <si>
+    <t>ولع</t>
+  </si>
+  <si>
+    <t>مؤسس</t>
+  </si>
+  <si>
+    <t>generation(n)</t>
+  </si>
+  <si>
+    <t>generous(adj)</t>
+  </si>
+  <si>
+    <t>جيل</t>
+  </si>
+  <si>
+    <t>كريم</t>
+  </si>
+  <si>
+    <t>inspire(d)(v)</t>
+  </si>
+  <si>
+    <t>instead(adv)</t>
+  </si>
+  <si>
+    <t>intelligence(adj)</t>
+  </si>
+  <si>
+    <t>iron level(n)</t>
+  </si>
+  <si>
+    <t>يلهم/أثر في</t>
+  </si>
+  <si>
+    <t>بدلاً من</t>
+  </si>
+  <si>
+    <t>ذكاء</t>
+  </si>
+  <si>
+    <t>مستوى الحديد</t>
+  </si>
+  <si>
+    <t>knowledge(n)</t>
+  </si>
+  <si>
+    <t>معرفة</t>
+  </si>
+  <si>
+    <t>long-term(adj)</t>
+  </si>
+  <si>
+    <t>طويل الأمد</t>
+  </si>
+  <si>
+    <t>maker(n)</t>
+  </si>
+  <si>
+    <t>movement(n)</t>
+  </si>
+  <si>
+    <t>name(d)(n-v)</t>
+  </si>
+  <si>
+    <t>صانع</t>
+  </si>
+  <si>
+    <t>حركة</t>
+  </si>
+  <si>
+    <t>nickname(n)</t>
+  </si>
+  <si>
+    <t>اسم</t>
+  </si>
+  <si>
+    <t>كنية/لقب</t>
+  </si>
+  <si>
+    <t>persuade(d)(v)</t>
+  </si>
+  <si>
+    <t>praise(d)(n-v)</t>
+  </si>
+  <si>
+    <t>purpose(n)</t>
+  </si>
+  <si>
+    <t>pressure(n)</t>
+  </si>
+  <si>
+    <t>prestige(n-adj)</t>
+  </si>
+  <si>
+    <t>يقنع</t>
+  </si>
+  <si>
+    <t>مدح</t>
+  </si>
+  <si>
+    <t>غرض</t>
+  </si>
+  <si>
+    <t>ضغط</t>
+  </si>
+  <si>
+    <t>هيبة</t>
+  </si>
+  <si>
+    <t>regular(adj)</t>
+  </si>
+  <si>
+    <t>relationship(n)</t>
+  </si>
+  <si>
+    <t>reduce(d)(v)</t>
+  </si>
+  <si>
+    <t>research(ed)(n-v)</t>
+  </si>
+  <si>
+    <t>respect(ed)(n-v)</t>
+  </si>
+  <si>
+    <t>role(n)</t>
+  </si>
+  <si>
+    <t>role play(n-v)</t>
+  </si>
+  <si>
+    <t>roar(ed)</t>
+  </si>
+  <si>
+    <t>role model</t>
+  </si>
+  <si>
+    <t>عادي/منتظم</t>
+  </si>
+  <si>
+    <t>علاقة</t>
+  </si>
+  <si>
+    <t>يقلل</t>
+  </si>
+  <si>
+    <t>بحث</t>
+  </si>
+  <si>
+    <t>احترام</t>
+  </si>
+  <si>
+    <t>دور</t>
+  </si>
+  <si>
+    <t>لعب دور</t>
+  </si>
+  <si>
+    <t>هدير/زئير</t>
+  </si>
+  <si>
+    <t>قدوة</t>
+  </si>
+  <si>
+    <t>save(d)(v)</t>
+  </si>
+  <si>
+    <t>score(d)(v-n)</t>
+  </si>
+  <si>
+    <t>speed(n)</t>
+  </si>
+  <si>
+    <t>support(ed)(n-v)</t>
+  </si>
+  <si>
+    <t>يحفظ</t>
+  </si>
+  <si>
+    <t>نتيجة</t>
+  </si>
+  <si>
+    <t>سرعة</t>
+  </si>
+  <si>
+    <t>يدعم</t>
+  </si>
+  <si>
+    <t>transplant(ed)(n-v)</t>
+  </si>
+  <si>
+    <t>زرع اعضاء</t>
+  </si>
+  <si>
+    <t>own(v)</t>
+  </si>
+  <si>
+    <t>ملك</t>
+  </si>
+  <si>
+    <t>يدين</t>
+  </si>
+  <si>
+    <t>owe(v)</t>
+  </si>
+  <si>
+    <t>extenction(n)</t>
+  </si>
+  <si>
+    <t>انقراض</t>
+  </si>
+  <si>
+    <t>scientists(n)</t>
+  </si>
+  <si>
+    <t>العلماء</t>
+  </si>
+  <si>
+    <t>encourage(v)</t>
+  </si>
+  <si>
+    <t>يشجع</t>
+  </si>
+  <si>
+    <t>cycling(n)</t>
+  </si>
+  <si>
+    <t>ركوب الدراجات</t>
+  </si>
+  <si>
+    <t>غير متجدد</t>
+  </si>
+  <si>
+    <t>nonrenewable(adj)</t>
+  </si>
+  <si>
+    <t>arise(v)</t>
+  </si>
+  <si>
+    <t>تنشأ</t>
+  </si>
+  <si>
+    <t>diseases(n)</t>
+  </si>
+  <si>
+    <t>الأمراض</t>
+  </si>
+  <si>
+    <t>nowadays(adv)</t>
+  </si>
+  <si>
+    <t>في الوقت الحاضر</t>
+  </si>
+  <si>
+    <t>laid(v)</t>
+  </si>
+  <si>
+    <t>وضع</t>
+  </si>
+  <si>
+    <t>robbed(v)</t>
+  </si>
+  <si>
+    <t>سرق شخص او مكان</t>
+  </si>
+  <si>
+    <t>يسرق شيء</t>
+  </si>
+  <si>
+    <t>injured(adj)</t>
+  </si>
+  <si>
+    <t>مصاب</t>
+  </si>
+  <si>
+    <t>clues(n)</t>
+  </si>
+  <si>
+    <t>أدلة</t>
+  </si>
+  <si>
+    <t>improve(v)</t>
+  </si>
+  <si>
+    <t>يحسن</t>
+  </si>
+  <si>
+    <t>admitting(n)</t>
+  </si>
+  <si>
+    <t>الاعتراف</t>
+  </si>
+  <si>
+    <t>غفر</t>
+  </si>
+  <si>
+    <t>forgave(v)</t>
+  </si>
+  <si>
+    <t>debt(n)</t>
+  </si>
+  <si>
+    <t>دَين</t>
+  </si>
+  <si>
+    <t>متحمس</t>
+  </si>
+  <si>
+    <t>interested(in)</t>
+  </si>
+  <si>
+    <t>مهتم</t>
+  </si>
+  <si>
+    <t>keen(on)(adj)</t>
+  </si>
+  <si>
+    <t>crutch(n)</t>
+  </si>
+  <si>
+    <t>عكاز</t>
+  </si>
+  <si>
+    <t>patient(adj)</t>
+  </si>
+  <si>
+    <t>صبور/مريض</t>
+  </si>
+  <si>
+    <t>rewarded</t>
+  </si>
+  <si>
+    <t>مكافأة</t>
+  </si>
+  <si>
+    <t>deserved(v)</t>
+  </si>
+  <si>
+    <t>استحق</t>
+  </si>
+  <si>
+    <t>miser(adj)</t>
+  </si>
+  <si>
+    <t>البخيل</t>
+  </si>
+  <si>
+    <t>tricks(n)</t>
+  </si>
+  <si>
+    <t>الخدع</t>
+  </si>
+  <si>
+    <t>تاجر</t>
+  </si>
+  <si>
+    <t>merchant(n)</t>
   </si>
 </sst>
 </file>
@@ -1028,15 +1508,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1077,7 +1557,7 @@
         <v>174</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,6 +1574,54 @@
       </c>
       <c r="B7" t="s">
         <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>220</v>
+      </c>
+      <c r="B9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>222</v>
+      </c>
+      <c r="B10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B12" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -1115,22 +1643,44 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FEDBBB-0740-434B-9266-B937B39AC021}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D22F8E0-D4FF-43F0-90F8-96ADC458F438}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1729,22 @@
         <v>144</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B7" t="s">
+        <v>347</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1186,14 +1752,15 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D50DDAE-F9E0-49CD-ABF9-66E050FDB604}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1211,6 +1778,38 @@
       </c>
       <c r="B2" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>281</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B6" t="s">
+        <v>379</v>
       </c>
     </row>
   </sheetData>
@@ -1220,13 +1819,17 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96ED2B6-26BB-4769-85D0-CC94C25BB600}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1234,6 +1837,38 @@
       </c>
       <c r="B1" t="s">
         <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>344</v>
+      </c>
+      <c r="B5" t="s">
+        <v>345</v>
       </c>
     </row>
   </sheetData>
@@ -1243,10 +1878,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C0C726-EF5B-4FC9-82F4-48A94ABEDF76}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,6 +1930,22 @@
         <v>197</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B7" t="s">
+        <v>328</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1302,15 +1953,15 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8A7C8CB-6C90-4DBF-A892-A597E3AA4FFB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1384,6 +2035,54 @@
       </c>
       <c r="B9" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>289</v>
+      </c>
+      <c r="B11" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>290</v>
+      </c>
+      <c r="B12" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>291</v>
+      </c>
+      <c r="B13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>369</v>
+      </c>
+      <c r="B15" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -1419,16 +2118,16 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B3BD8CC-E8BB-4467-BDFA-859B668822CD}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1477,6 +2176,94 @@
       </c>
       <c r="B6" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>301</v>
+      </c>
+      <c r="B10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>303</v>
+      </c>
+      <c r="B12" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>304</v>
+      </c>
+      <c r="B13" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>306</v>
+      </c>
+      <c r="B15" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -1486,10 +2273,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC3E5B7-A644-40B3-9FA0-0F3184C0C666}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,15 +2362,55 @@
         <v>204</v>
       </c>
       <c r="B10" t="s">
-        <v>205</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B11" t="s">
         <v>206</v>
       </c>
-      <c r="B11" t="s">
-        <v>207</v>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>316</v>
+      </c>
+      <c r="B12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>317</v>
+      </c>
+      <c r="B13" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>318</v>
+      </c>
+      <c r="B14" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>319</v>
+      </c>
+      <c r="B15" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>332</v>
+      </c>
+      <c r="B16" t="s">
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -1593,15 +2420,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{853577DC-45D1-47FB-8CE1-2701635EB942}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1650,6 +2478,46 @@
       </c>
       <c r="B6" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>231</v>
+      </c>
+      <c r="B10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -1659,15 +2527,15 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB031BE2-8873-4BBE-A6E2-D6DA83495605}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1681,18 +2549,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" t="s">
         <v>208</v>
-      </c>
-      <c r="B2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" t="s">
         <v>210</v>
       </c>
-      <c r="B3" t="s">
-        <v>211</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>377</v>
+      </c>
+      <c r="B5" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -1723,18 +2607,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" t="s">
         <v>212</v>
-      </c>
-      <c r="B2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B3" t="s">
         <v>214</v>
-      </c>
-      <c r="B3" t="s">
-        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1807,10 +2691,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -1832,10 +2716,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C22D18F6-24F4-4B6D-89D6-327046526B24}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,6 +2816,70 @@
         <v>178</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B12" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>239</v>
+      </c>
+      <c r="B13" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>240</v>
+      </c>
+      <c r="B14" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>241</v>
+      </c>
+      <c r="B15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>242</v>
+      </c>
+      <c r="B16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>353</v>
+      </c>
+      <c r="B18" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B19" t="s">
+        <v>368</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1939,15 +2887,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620BC664-2145-4DF7-8DD0-BC60C18F3A8C}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2005,6 +2953,70 @@
       </c>
       <c r="B7" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>249</v>
+      </c>
+      <c r="B9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B11" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>252</v>
+      </c>
+      <c r="B12" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>361</v>
+      </c>
+      <c r="B14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>373</v>
+      </c>
+      <c r="B15" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -2014,10 +3026,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ED53159-19AE-4D6E-99FF-244D3305644D}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2138,6 +3150,22 @@
         <v>185</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>330</v>
+      </c>
+      <c r="B15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>334</v>
+      </c>
+      <c r="B16" t="s">
+        <v>335</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2145,10 +3173,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAE4078B-C3FB-4387-BB88-A48544D11CEB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2173,6 +3201,38 @@
         <v>187</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>260</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" t="s">
+        <v>359</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2180,10 +3240,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40C90A18-1FDE-4DAE-9E49-D28AE616AC3A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2229,6 +3289,22 @@
       </c>
       <c r="B5" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B6" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B7" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -2272,10 +3348,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CE4CAFB-C354-4385-8BA3-69100390E382}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2326,10 +3402,66 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" t="s">
         <v>219</v>
       </c>
-      <c r="B6" t="s">
-        <v>220</v>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B8" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>270</v>
+      </c>
+      <c r="B9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>355</v>
+      </c>
+      <c r="B12" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>